<commit_message>
LTSpice simulation of the N555 model. Open for changes
</commit_message>
<xml_diff>
--- a/Lanna/Material Analysis.xlsx
+++ b/Lanna/Material Analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lagas\ec209-project-2024_team_11\310TEAM11\Lanna\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5e9f6f23649702a4/ELECTENG310/310TEAM11/Lanna/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{DF24A679-3586-4B13-9A68-7C8616DD3148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E376315D-3DEC-4A55-85A5-99239D792156}"/>
+    <workbookView minimized="1" xWindow="2010" yWindow="1020" windowWidth="8330" windowHeight="3880" xr2:uid="{E376315D-3DEC-4A55-85A5-99239D792156}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -293,7 +293,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-NZ"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -567,7 +567,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NZ"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1672,7 +1672,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -5450,18 +5449,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC4A8D4-A82C-4877-8D73-28FAA28BD9D2}">
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="13" max="17" width="11.28515625" customWidth="1"/>
+    <col min="1" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="13" max="17" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -5481,7 +5480,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="M2" s="1">
         <f>1.2993*10^-13</f>
         <v>1.2992999999999998E-13</v>
@@ -5494,7 +5493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <f>1.2993*10^-13</f>
         <v>1.2992999999999998E-13</v>
@@ -5518,7 +5517,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <f>8.1207*10^-11</f>
         <v>8.1206999999999984E-11</v>
@@ -5542,7 +5541,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <f>1.6242*10^-10</f>
         <v>1.6242000000000002E-10</v>
@@ -5566,7 +5565,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <f>2.4362*10^-10</f>
         <v>2.4361999999999998E-10</v>
@@ -5590,7 +5589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <f>3.2483*10^-10</f>
         <v>3.2483E-10</v>
@@ -5603,7 +5602,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -5629,7 +5628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <f>5.6156*10^-14</f>
         <v>5.6155999999999998E-14</v>
@@ -5657,7 +5656,7 @@
         <v>1.4458400000000001E-13</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <f>3.5098*10^-11</f>
         <v>3.5097999999999996E-11</v>
@@ -5684,7 +5683,7 @@
         <v>9.0365000000000003E-11</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <f>7.0196*10^-11</f>
         <v>7.0195999999999992E-11</v>
@@ -5711,7 +5710,7 @@
         <v>1.8073000000000001E-10</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <f>1.0529*10^-10</f>
         <v>1.0528999999999999E-10</v>
@@ -5738,7 +5737,7 @@
         <v>2.7109540000000001E-10</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <f>1.4039*10^-10</f>
         <v>1.4038999999999999E-10</v>

</xml_diff>